<commit_message>
Docs: Se añade Historias de Usuario (Clientes)
</commit_message>
<xml_diff>
--- a/Primer Trimestre/Historias de Usuario/Historias de usuario.xlsx
+++ b/Primer Trimestre/Historias de Usuario/Historias de usuario.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo M72\Downloads\SENA 2021\Tarea 17022021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo M72\Downloads\SENA 2021\PROYECTO\Historias de Usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8535"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cliente" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -336,6 +336,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -353,9 +356,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -640,7 +640,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,18 +656,18 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -699,16 +699,16 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="16" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="2">
@@ -728,10 +728,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
       <c r="E4" s="2">
         <v>2</v>
       </c>
@@ -760,16 +760,16 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="16" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="2">
@@ -789,10 +789,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="2">
         <v>2</v>
       </c>
@@ -821,16 +821,16 @@
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="2">
@@ -850,10 +850,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="2">
         <v>2</v>
       </c>
@@ -920,16 +920,16 @@
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="18" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="2">
@@ -949,10 +949,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="18"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="2">
         <v>2</v>
       </c>
@@ -982,12 +982,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
@@ -1000,6 +994,12 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>